<commit_message>
adding interest rate data
</commit_message>
<xml_diff>
--- a/data/infl_interest.xlsx
+++ b/data/infl_interest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/ExchangeRatePrediction/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C31AB86C-6C0D-964B-8F2D-98C51E573BA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E262515B-4870-E249-A388-D984E1A1F7B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="125">
   <si>
     <t>Development relevance</t>
   </si>
@@ -305,9 +305,6 @@
     <t>FR.INR.RINR</t>
   </si>
   <si>
-    <t>Series Code</t>
-  </si>
-  <si>
     <t>2010 [YR2010]</t>
   </si>
   <si>
@@ -407,6 +404,9 @@
     <t>The banking system's assets include its net foreign assets and net domestic credit. Net domestic credit includes credit extended to the private sector and general government and credit extended to the nonfinancial public sector in the form of investments in short- and long-term government securities and loans to state enterprises; liabilities to the public and private sectors in the form of deposits with the banking system are netted out. Net domestic credit also includes credit to banking and nonbank financial institutions.
 Domestic credit is the main vehicle through which changes in the money supply are regulated, with central bank lending to the government often playing the most important role. The central bank can regulate lending to the private sector in several ways - for example, by adjusting the cost of the refinancing facilities it provides to banks, by changing market interest rates through open market operations, or by controlling the availability of credit through changes in the reserve requirements imposed on banks and ceilings on the credit provided by banks to the private sector.
 The real interest rate is used in various economic theories to explain such phenomena as the capital flight, business cycle and economic bubbles. When the real rate of interest is high, that is, demand for credit is high, then money will, all other things being equal, move from consumption to savings. Conversely, when the real rate of interest is low, demand will move from savings to investment and consumption.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -748,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BB18"/>
+  <dimension ref="A1:BA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y19" sqref="Y19"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -761,7 +761,7 @@
     <col min="3" max="3" width="43.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -769,163 +769,160 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" t="s">
+        <v>96</v>
+      </c>
+      <c r="W1" t="s">
+        <v>84</v>
+      </c>
+      <c r="X1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ1" t="s">
         <v>91</v>
       </c>
-      <c r="E1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" t="s">
-        <v>117</v>
-      </c>
-      <c r="N1" t="s">
-        <v>101</v>
-      </c>
-      <c r="O1" t="s">
-        <v>89</v>
-      </c>
-      <c r="P1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S1" t="s">
-        <v>62</v>
-      </c>
-      <c r="T1" t="s">
-        <v>54</v>
-      </c>
-      <c r="U1" t="s">
-        <v>45</v>
-      </c>
-      <c r="V1" t="s">
-        <v>33</v>
-      </c>
-      <c r="W1" t="s">
-        <v>97</v>
-      </c>
-      <c r="X1" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>121</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>103</v>
-      </c>
       <c r="AR1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="AS1" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="AT1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="AU1" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="AV1" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="AW1" t="s">
-        <v>107</v>
+        <v>46</v>
       </c>
       <c r="AX1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="AY1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="AZ1" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="BA1" t="s">
-        <v>85</v>
-      </c>
-      <c r="BB1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -935,161 +932,158 @@
       <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
+      <c r="D2">
+        <v>1.7610062893081899</v>
       </c>
       <c r="E2">
-        <v>1.7610062893081899</v>
+        <v>2.0807581376187798</v>
       </c>
       <c r="F2">
-        <v>2.0807581376187798</v>
+        <v>19.6367305751765</v>
       </c>
       <c r="G2">
-        <v>19.6367305751765</v>
+        <v>22.368421052631501</v>
       </c>
       <c r="H2">
-        <v>22.368421052631501</v>
+        <v>2.5365315687894898</v>
       </c>
       <c r="I2">
-        <v>2.5365315687894898</v>
+        <v>-1.84189298198423</v>
       </c>
       <c r="J2">
-        <v>-1.84189298198423</v>
+        <v>3.1639501438158399</v>
       </c>
       <c r="K2">
-        <v>3.1639501438158399</v>
+        <v>4.87254381306425</v>
       </c>
       <c r="L2">
-        <v>4.87254381306425</v>
+        <v>4.0764653753639903</v>
       </c>
       <c r="M2">
-        <v>4.0764653753639903</v>
+        <v>8.5269431942585907</v>
       </c>
       <c r="N2">
-        <v>8.5269431942585907</v>
+        <v>8.1820219681684794</v>
       </c>
       <c r="O2">
-        <v>8.1820219681684794</v>
+        <v>3.91628677994199</v>
       </c>
       <c r="P2">
-        <v>3.91628677994199</v>
+        <v>1.19641076769694</v>
       </c>
       <c r="Q2">
-        <v>1.19641076769694</v>
+        <v>2.6009852216748501</v>
       </c>
       <c r="R2">
-        <v>2.6009852216748501</v>
+        <v>0.48012291146535202</v>
       </c>
       <c r="S2">
-        <v>0.48012291146535202</v>
+        <v>-1.38570336391444</v>
       </c>
       <c r="T2">
-        <v>-1.38570336391444</v>
+        <v>0.52330652194980498</v>
       </c>
       <c r="U2">
-        <v>0.52330652194980498</v>
+        <v>1.5231851923263</v>
       </c>
       <c r="V2">
-        <v>1.5231851923263</v>
+        <v>2.34545627195899</v>
       </c>
       <c r="W2">
-        <v>2.34545627195899</v>
+        <v>3.4607533865282099</v>
       </c>
       <c r="X2">
-        <v>3.4607533865282099</v>
+        <v>3.4257017307864399</v>
       </c>
       <c r="Y2">
-        <v>3.4257017307864399</v>
+        <v>2.2630711870284901</v>
       </c>
       <c r="Z2">
-        <v>2.2630711870284901</v>
+        <v>2.2892996438864199</v>
       </c>
       <c r="AA2">
-        <v>2.2892996438864199</v>
+        <v>3.1001326259950299</v>
       </c>
       <c r="AB2">
-        <v>3.1001326259950299</v>
+        <v>1.7205338478852401</v>
       </c>
       <c r="AC2">
-        <v>1.7205338478852401</v>
+        <v>1.3831805248187801</v>
       </c>
       <c r="AD2">
-        <v>1.3831805248187801</v>
+        <v>2.00358618538958</v>
       </c>
       <c r="AE2">
-        <v>2.00358618538958</v>
+        <v>-0.26750229287612698</v>
       </c>
       <c r="AF2">
-        <v>-0.26750229287612698</v>
+        <v>1.6709833737075901E-2</v>
       </c>
       <c r="AG2">
-        <v>1.6709833737075901E-2</v>
+        <v>1.3616239244845501</v>
       </c>
       <c r="AH2">
-        <v>1.3616239244845501</v>
+        <v>0.99719795615596696</v>
       </c>
       <c r="AI2">
-        <v>0.99719795615596696</v>
+        <v>-0.391676866585079</v>
       </c>
       <c r="AJ2">
-        <v>-0.391676866585079</v>
+        <v>0.50790530023753899</v>
       </c>
       <c r="AK2">
-        <v>0.50790530023753899</v>
+        <v>1.6627271986307299</v>
       </c>
       <c r="AL2">
-        <v>1.6627271986307299</v>
+        <v>0.42510627656910099</v>
       </c>
       <c r="AM2">
-        <v>0.42510627656910099</v>
+        <v>0.96290177816512801</v>
       </c>
       <c r="AN2">
-        <v>0.96290177816512801</v>
+        <v>2.1048800363321298</v>
       </c>
       <c r="AO2">
-        <v>2.1048800363321298</v>
+        <v>6.6277817735212698</v>
       </c>
       <c r="AP2">
-        <v>6.6277817735212698</v>
+        <v>0.59672025742497203</v>
       </c>
       <c r="AQ2">
-        <v>0.59672025742497203</v>
+        <v>2.8236613488560902</v>
       </c>
       <c r="AR2">
-        <v>2.8236613488560902</v>
+        <v>5.2477933984048004</v>
       </c>
       <c r="AS2">
-        <v>5.2477933984048004</v>
+        <v>4.5756027037652203</v>
       </c>
       <c r="AT2">
-        <v>4.5756027037652203</v>
+        <v>2.35860415399836</v>
       </c>
       <c r="AU2">
-        <v>2.35860415399836</v>
+        <v>1.02514803039394</v>
       </c>
       <c r="AV2">
-        <v>1.02514803039394</v>
+        <v>-0.52261816707531406</v>
       </c>
       <c r="AW2">
-        <v>-0.52261816707531406</v>
+        <v>-0.53226873971628996</v>
       </c>
       <c r="AX2">
-        <v>-0.53226873971628996</v>
+        <v>0.57626031016637103</v>
       </c>
       <c r="AY2">
-        <v>0.57626031016637103</v>
+        <v>0.438620118446782</v>
       </c>
       <c r="AZ2">
-        <v>0.438620118446782</v>
-      </c>
-      <c r="BA2">
         <v>0.56526056878035802</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BA2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -1099,161 +1093,158 @@
       <c r="C3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>24</v>
+      <c r="D3">
+        <v>12.413755064382855</v>
       </c>
       <c r="E3">
-        <v>12.413755064382855</v>
+        <v>13.315550718367078</v>
       </c>
       <c r="F3">
-        <v>13.315550718367078</v>
+        <v>10.602619262245085</v>
       </c>
       <c r="G3">
-        <v>10.602619262245085</v>
+        <v>6.117604350549513</v>
       </c>
       <c r="H3">
-        <v>6.117604350549513</v>
+        <v>3.9816879915482986</v>
       </c>
       <c r="I3">
-        <v>3.9816879915482986</v>
+        <v>7.4371768530852762</v>
       </c>
       <c r="J3">
-        <v>7.4371768530852762</v>
+        <v>6.8526996802713995</v>
       </c>
       <c r="K3">
-        <v>6.8526996802713995</v>
+        <v>7.7772876565305182</v>
       </c>
       <c r="L3">
-        <v>7.7772876565305182</v>
+        <v>9.5541733359054462</v>
       </c>
       <c r="M3">
-        <v>9.5541733359054462</v>
+        <v>10.113217783615553</v>
       </c>
       <c r="N3">
-        <v>10.113217783615553</v>
+        <v>10.81613733460398</v>
       </c>
       <c r="O3">
-        <v>10.81613733460398</v>
+        <v>7.1021148389738755</v>
       </c>
       <c r="P3">
-        <v>7.1021148389738755</v>
+        <v>8.5545996631617243</v>
       </c>
       <c r="Q3">
-        <v>8.5545996631617243</v>
+        <v>8.792386562430309</v>
       </c>
       <c r="R3">
-        <v>8.792386562430309</v>
+        <v>-0.62285124030650252</v>
       </c>
       <c r="S3">
-        <v>-0.62285124030650252</v>
+        <v>1.3428691105974195</v>
       </c>
       <c r="T3">
-        <v>1.3428691105974195</v>
+        <v>10.797769905977248</v>
       </c>
       <c r="U3">
-        <v>10.797769905977248</v>
+        <v>11.263750687361679</v>
       </c>
       <c r="V3">
-        <v>11.263750687361679</v>
+        <v>10.158610318797685</v>
       </c>
       <c r="W3">
-        <v>10.158610318797685</v>
+        <v>9.8210491311723871</v>
       </c>
       <c r="X3">
-        <v>9.8210491311723871</v>
+        <v>6.6885025132436908</v>
       </c>
       <c r="Y3">
-        <v>6.6885025132436908</v>
+        <v>6.6396895904467783</v>
       </c>
       <c r="Z3">
-        <v>6.6396895904467783</v>
+        <v>11.46277473940242</v>
       </c>
       <c r="AA3">
-        <v>11.46277473940242</v>
+        <v>11.097647937746743</v>
       </c>
       <c r="AB3">
-        <v>11.097647937746743</v>
+        <v>7.2009074900715859</v>
       </c>
       <c r="AC3">
-        <v>7.2009074900715859</v>
+        <v>7.4713795903942781</v>
       </c>
       <c r="AD3">
-        <v>7.4713795903942781</v>
+        <v>8.3199165270180515</v>
       </c>
       <c r="AE3">
-        <v>8.3199165270180515</v>
+        <v>-2.1953778262461014</v>
       </c>
       <c r="AF3">
-        <v>-2.1953778262461014</v>
+        <v>5.7240084235055946</v>
       </c>
       <c r="AG3">
-        <v>5.7240084235055946</v>
+        <v>9.0391467513396293</v>
       </c>
       <c r="AH3">
-        <v>9.0391467513396293</v>
+        <v>-1.0690158850810434</v>
       </c>
       <c r="AI3">
-        <v>-1.0690158850810434</v>
+        <v>3.9146097454129745</v>
       </c>
       <c r="AJ3">
-        <v>3.9146097454129745</v>
+        <v>4.5357796538632442</v>
       </c>
       <c r="AK3">
-        <v>4.5357796538632442</v>
+        <v>9.8195916770496439</v>
       </c>
       <c r="AL3">
-        <v>9.8195916770496439</v>
+        <v>7.3590336771345335</v>
       </c>
       <c r="AM3">
-        <v>7.3590336771345335</v>
+        <v>9.0051437297945967</v>
       </c>
       <c r="AN3">
-        <v>9.0051437297945967</v>
+        <v>9.0221330140232965</v>
       </c>
       <c r="AO3">
-        <v>9.0221330140232965</v>
+        <v>1.8682455341607351</v>
       </c>
       <c r="AP3">
-        <v>1.8682455341607351</v>
+        <v>0.1209827417308702</v>
       </c>
       <c r="AQ3">
-        <v>0.1209827417308702</v>
+        <v>14.525638994062717</v>
       </c>
       <c r="AR3">
-        <v>14.525638994062717</v>
+        <v>6.3378708138408086</v>
       </c>
       <c r="AS3">
-        <v>6.3378708138408086</v>
+        <v>4.4616089510133321</v>
       </c>
       <c r="AT3">
-        <v>4.4616089510133321</v>
+        <v>4.837298645760967</v>
       </c>
       <c r="AU3">
-        <v>4.837298645760967</v>
+        <v>3.9380027286605639</v>
       </c>
       <c r="AV3">
-        <v>3.9380027286605639</v>
+        <v>2.988520675577135</v>
       </c>
       <c r="AW3">
-        <v>2.988520675577135</v>
+        <v>3.2434741681369701</v>
       </c>
       <c r="AX3">
-        <v>3.2434741681369701</v>
+        <v>4.336604919181724</v>
       </c>
       <c r="AY3">
-        <v>4.336604919181724</v>
+        <v>3.4381110416144622</v>
       </c>
       <c r="AZ3">
-        <v>3.4381110416144622</v>
-      </c>
-      <c r="BA3">
         <v>0.73330993455972759</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="BA3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -1261,10 +1252,10 @@
         <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
       </c>
       <c r="E4" t="s">
         <v>31</v>
@@ -1284,98 +1275,98 @@
       <c r="J4" t="s">
         <v>31</v>
       </c>
-      <c r="K4" t="s">
-        <v>31</v>
+      <c r="K4">
+        <v>7.17</v>
       </c>
       <c r="L4">
-        <v>7.17</v>
+        <v>8.5033333330000005</v>
       </c>
       <c r="M4">
-        <v>8.5033333330000005</v>
+        <v>11.721666666000001</v>
       </c>
       <c r="N4">
-        <v>11.721666666000001</v>
+        <v>13.645</v>
       </c>
       <c r="O4">
-        <v>13.645</v>
+        <v>10.228333333</v>
       </c>
       <c r="P4">
-        <v>10.228333333</v>
+        <v>9.0508333333333297</v>
       </c>
       <c r="Q4">
-        <v>9.0508333333333297</v>
+        <v>9.7191666666666698</v>
       </c>
       <c r="R4">
-        <v>9.7191666666666698</v>
+        <v>8.0641666666666705</v>
       </c>
       <c r="S4">
-        <v>8.0641666666666705</v>
+        <v>6.82</v>
       </c>
       <c r="T4">
-        <v>6.82</v>
+        <v>6.1</v>
       </c>
       <c r="U4">
-        <v>6.1</v>
+        <v>5.9641666666666699</v>
       </c>
       <c r="V4">
-        <v>5.9641666666666699</v>
+        <v>6.2116666666666696</v>
       </c>
       <c r="W4">
-        <v>6.2116666666666696</v>
+        <v>7.3624999999999998</v>
       </c>
       <c r="X4">
-        <v>7.3624999999999998</v>
+        <v>7.5833333333333304</v>
       </c>
       <c r="Y4">
-        <v>7.5833333333333304</v>
+        <v>5.9524999999999997</v>
       </c>
       <c r="Z4">
-        <v>5.9524999999999997</v>
+        <v>5.3883333333333301</v>
       </c>
       <c r="AA4">
-        <v>5.3883333333333301</v>
+        <v>5.8783333333333303</v>
       </c>
       <c r="AB4">
-        <v>5.8783333333333303</v>
+        <v>6.3691666666666604</v>
       </c>
       <c r="AC4">
-        <v>6.3691666666666604</v>
+        <v>6.26</v>
       </c>
       <c r="AD4">
-        <v>6.26</v>
+        <v>6.3224999999999998</v>
       </c>
       <c r="AE4">
-        <v>6.3224999999999998</v>
+        <v>7.4416666666666602</v>
       </c>
       <c r="AF4">
-        <v>7.4416666666666602</v>
+        <v>5.8</v>
       </c>
       <c r="AG4">
-        <v>5.8</v>
+        <v>5.8333333333333304</v>
       </c>
       <c r="AH4">
-        <v>5.8333333333333304</v>
+        <v>5.6483333333333299</v>
       </c>
       <c r="AI4">
-        <v>5.6483333333333299</v>
+        <v>5.3458333333333297</v>
       </c>
       <c r="AJ4">
-        <v>5.3458333333333297</v>
+        <v>5.3066666666666702</v>
       </c>
       <c r="AK4">
-        <v>5.3066666666666702</v>
+        <v>5.3</v>
       </c>
       <c r="AL4">
         <v>5.3</v>
       </c>
       <c r="AM4">
-        <v>5.3</v>
+        <v>5.3125</v>
       </c>
       <c r="AN4">
-        <v>5.3125</v>
+        <v>5.33</v>
       </c>
       <c r="AO4">
-        <v>5.33</v>
+        <v>5.38</v>
       </c>
       <c r="AP4">
         <v>5.38</v>
@@ -1393,7 +1384,7 @@
         <v>5.38</v>
       </c>
       <c r="AU4">
-        <v>5.38</v>
+        <v>5.35</v>
       </c>
       <c r="AV4">
         <v>5.35</v>
@@ -1402,22 +1393,19 @@
         <v>5.35</v>
       </c>
       <c r="AX4">
-        <v>5.35</v>
+        <v>5.28</v>
       </c>
       <c r="AY4">
-        <v>5.28</v>
+        <v>5.33</v>
       </c>
       <c r="AZ4">
-        <v>5.33</v>
+        <v>5.25</v>
       </c>
       <c r="BA4">
         <v>5.25</v>
       </c>
-      <c r="BB4">
-        <v>5.25</v>
-      </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1427,8 +1415,8 @@
       <c r="C5" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>90</v>
+      <c r="D5" t="s">
+        <v>31</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1448,140 +1436,137 @@
       <c r="J5" t="s">
         <v>31</v>
       </c>
-      <c r="K5" t="s">
-        <v>31</v>
+      <c r="K5">
+        <v>3.0066991154126343</v>
       </c>
       <c r="L5">
-        <v>3.0066991154126343</v>
+        <v>3.1050958359716043</v>
       </c>
       <c r="M5">
-        <v>3.1050958359716043</v>
+        <v>0.5348839626496199</v>
       </c>
       <c r="N5">
-        <v>0.5348839626496199</v>
+        <v>7.3385541781879304</v>
       </c>
       <c r="O5">
-        <v>7.3385541781879304</v>
+        <v>5.4483745408399065</v>
       </c>
       <c r="P5">
-        <v>5.4483745408399065</v>
+        <v>5.6987784584370296</v>
       </c>
       <c r="Q5">
-        <v>5.6987784584370296</v>
+        <v>8.861526159659407</v>
       </c>
       <c r="R5">
-        <v>8.861526159659407</v>
+        <v>9.6712179455271574</v>
       </c>
       <c r="S5">
-        <v>9.6712179455271574</v>
+        <v>8.1752990929821756</v>
       </c>
       <c r="T5">
-        <v>8.1752990929821756</v>
+        <v>5.5379308955232851</v>
       </c>
       <c r="U5">
-        <v>5.5379308955232851</v>
+        <v>0.50611088001218929</v>
       </c>
       <c r="V5">
-        <v>0.50611088001218929</v>
+        <v>1.9703360556895593</v>
       </c>
       <c r="W5">
-        <v>1.9703360556895593</v>
+        <v>2.545643279417936</v>
       </c>
       <c r="X5">
-        <v>2.545643279417936</v>
+        <v>3.0143951460986491</v>
       </c>
       <c r="Y5">
-        <v>3.0143951460986491</v>
+        <v>4.5022044795928773</v>
       </c>
       <c r="Z5">
-        <v>4.5022044795928773</v>
+        <v>1.8704538829504989</v>
       </c>
       <c r="AA5">
-        <v>1.8704538829504989</v>
+        <v>2.336551650930391</v>
       </c>
       <c r="AB5">
-        <v>2.336551650930391</v>
+        <v>3.1191305848823179</v>
       </c>
       <c r="AC5">
-        <v>3.1191305848823179</v>
+        <v>4.6832262234740245</v>
       </c>
       <c r="AD5">
-        <v>4.6832262234740245</v>
+        <v>5.1848912905019873</v>
       </c>
       <c r="AE5">
-        <v>5.1848912905019873</v>
+        <v>8.8837746412810485</v>
       </c>
       <c r="AF5">
-        <v>8.8837746412810485</v>
+        <v>9.7316527598434064</v>
       </c>
       <c r="AG5">
-        <v>9.7316527598434064</v>
+        <v>1.897357838894439</v>
       </c>
       <c r="AH5">
-        <v>1.897357838894439</v>
+        <v>7.6026828579397883</v>
       </c>
       <c r="AI5">
-        <v>7.6026828579397883</v>
+        <v>6.2902968181721253</v>
       </c>
       <c r="AJ5">
-        <v>6.2902968181721253</v>
+        <v>7.2230962942780303</v>
       </c>
       <c r="AK5">
-        <v>7.2230962942780303</v>
+        <v>1.1784988435599735</v>
       </c>
       <c r="AL5">
-        <v>1.1784988435599735</v>
+        <v>3.3290634377968167</v>
       </c>
       <c r="AM5">
-        <v>3.3290634377968167</v>
+        <v>3.4039741069668108</v>
       </c>
       <c r="AN5">
-        <v>3.4039741069668108</v>
+        <v>-0.55348312385717569</v>
       </c>
       <c r="AO5">
-        <v>-0.55348312385717569</v>
+        <v>6.8612742136426181</v>
       </c>
       <c r="AP5">
-        <v>6.8612742136426181</v>
+        <v>2.3493413098217015</v>
       </c>
       <c r="AQ5">
-        <v>2.3493413098217015</v>
+        <v>4.2307420209540005</v>
       </c>
       <c r="AR5">
-        <v>4.2307420209540005</v>
+        <v>4.2810496096116504</v>
       </c>
       <c r="AS5">
-        <v>4.2810496096116504</v>
+        <v>4.8867952007091136</v>
       </c>
       <c r="AT5">
-        <v>4.8867952007091136</v>
+        <v>5.8560757320371843</v>
       </c>
       <c r="AU5">
-        <v>5.8560757320371843</v>
+        <v>5.6348262070810611</v>
       </c>
       <c r="AV5">
-        <v>5.6348262070810611</v>
+        <v>2.2217842666273948</v>
       </c>
       <c r="AW5">
-        <v>2.2217842666273948</v>
+        <v>4.6225359151438958</v>
       </c>
       <c r="AX5">
-        <v>4.6225359151438958</v>
+        <v>2.4320341124348941</v>
       </c>
       <c r="AY5">
-        <v>2.4320341124348941</v>
+        <v>2.1735230823520864</v>
       </c>
       <c r="AZ5">
-        <v>2.1735230823520864</v>
-      </c>
-      <c r="BA5">
         <v>5.1502481304091932</v>
       </c>
-      <c r="BB5" t="s">
+      <c r="BA5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -1591,8 +1576,8 @@
       <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>109</v>
+      <c r="D6" t="s">
+        <v>31</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
@@ -1615,137 +1600,134 @@
       <c r="K6" t="s">
         <v>31</v>
       </c>
-      <c r="L6" t="s">
-        <v>31</v>
+      <c r="L6">
+        <v>96.257211589211806</v>
       </c>
       <c r="M6">
-        <v>96.257211589211806</v>
+        <v>95.910450085239603</v>
       </c>
       <c r="N6">
-        <v>95.910450085239603</v>
+        <v>101.421226426882</v>
       </c>
       <c r="O6">
-        <v>101.421226426882</v>
+        <v>106.358682455991</v>
       </c>
       <c r="P6">
-        <v>106.358682455991</v>
+        <v>107.679185377868</v>
       </c>
       <c r="Q6">
-        <v>107.679185377868</v>
+        <v>109.435721789596</v>
       </c>
       <c r="R6">
-        <v>109.435721789596</v>
+        <v>106.73597677750099</v>
       </c>
       <c r="S6">
-        <v>106.73597677750099</v>
+        <v>91.013316658203095</v>
       </c>
       <c r="T6">
-        <v>91.013316658203095</v>
+        <v>85.4210230492439</v>
       </c>
       <c r="U6">
-        <v>85.4210230492439</v>
+        <v>83.738493930640601</v>
       </c>
       <c r="V6">
-        <v>83.738493930640601</v>
+        <v>87.511249425753405</v>
       </c>
       <c r="W6">
-        <v>87.511249425753405</v>
+        <v>93.037642943130805</v>
       </c>
       <c r="X6">
-        <v>93.037642943130805</v>
+        <v>96.061285446417102</v>
       </c>
       <c r="Y6">
-        <v>96.061285446417102</v>
+        <v>97.726926285293601</v>
       </c>
       <c r="Z6">
-        <v>97.726926285293601</v>
+        <v>98.004114207418596</v>
       </c>
       <c r="AA6">
-        <v>98.004114207418596</v>
+        <v>102.527400239465</v>
       </c>
       <c r="AB6">
-        <v>102.527400239465</v>
+        <v>104.27064384133899</v>
       </c>
       <c r="AC6">
-        <v>104.27064384133899</v>
+        <v>107.220798468344</v>
       </c>
       <c r="AD6">
-        <v>107.220798468344</v>
+        <v>108.563666245166</v>
       </c>
       <c r="AE6">
-        <v>108.563666245166</v>
+        <v>105.894250209302</v>
       </c>
       <c r="AF6">
-        <v>105.894250209302</v>
+        <v>98.680486449398401</v>
       </c>
       <c r="AG6">
-        <v>98.680486449398401</v>
+        <v>98.521616419120093</v>
       </c>
       <c r="AH6">
-        <v>98.521616419120093</v>
+        <v>99.037080047270905</v>
       </c>
       <c r="AI6">
-        <v>99.037080047270905</v>
+        <v>96.461674331576603</v>
       </c>
       <c r="AJ6">
-        <v>96.461674331576603</v>
+        <v>93.0750040519642</v>
       </c>
       <c r="AK6">
-        <v>93.0750040519642</v>
+        <v>92.030723438075896</v>
       </c>
       <c r="AL6">
-        <v>92.030723438075896</v>
+        <v>90.605488885533106</v>
       </c>
       <c r="AM6">
-        <v>90.605488885533106</v>
+        <v>91.824199035676898</v>
       </c>
       <c r="AN6">
-        <v>91.824199035676898</v>
+        <v>92.251350958564203</v>
       </c>
       <c r="AO6">
-        <v>92.251350958564203</v>
+        <v>97.026116005089506</v>
       </c>
       <c r="AP6">
-        <v>97.026116005089506</v>
+        <v>97.0344379377904</v>
       </c>
       <c r="AQ6">
-        <v>97.0344379377904</v>
+        <v>100</v>
       </c>
       <c r="AR6">
-        <v>100</v>
+        <v>105.174921402328</v>
       </c>
       <c r="AS6">
-        <v>105.174921402328</v>
+        <v>110.044835403528</v>
       </c>
       <c r="AT6">
-        <v>110.044835403528</v>
+        <v>112.0243164626</v>
       </c>
       <c r="AU6">
-        <v>112.0243164626</v>
+        <v>111.314060590167</v>
       </c>
       <c r="AV6">
-        <v>111.314060590167</v>
+        <v>108.323833740087</v>
       </c>
       <c r="AW6">
-        <v>108.323833740087</v>
+        <v>108.103365795074</v>
       </c>
       <c r="AX6">
-        <v>108.103365795074</v>
+        <v>106.812936405736</v>
       </c>
       <c r="AY6">
-        <v>106.812936405736</v>
+        <v>106.19868536046999</v>
       </c>
       <c r="AZ6">
-        <v>106.19868536046999</v>
-      </c>
-      <c r="BA6">
         <v>106.308013776327</v>
       </c>
-      <c r="BB6" t="s">
+      <c r="BA6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -1753,163 +1735,160 @@
         <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="D7">
+        <v>31.261628771961799</v>
       </c>
       <c r="E7">
-        <v>31.261628771961799</v>
+        <v>31.912107656586599</v>
       </c>
       <c r="F7">
-        <v>31.912107656586599</v>
+        <v>38.178602257970702</v>
       </c>
       <c r="G7">
-        <v>38.178602257970702</v>
+        <v>46.7185527630431</v>
       </c>
       <c r="H7">
-        <v>46.7185527630431</v>
+        <v>47.903583602359298</v>
       </c>
       <c r="I7">
-        <v>47.903583602359298</v>
+        <v>47.021250857868502</v>
       </c>
       <c r="J7">
-        <v>47.021250857868502</v>
+        <v>48.508979792010003</v>
       </c>
       <c r="K7">
-        <v>48.508979792010003</v>
+        <v>50.872601085646203</v>
       </c>
       <c r="L7">
-        <v>50.872601085646203</v>
+        <v>52.946405054449599</v>
       </c>
       <c r="M7">
-        <v>52.946405054449599</v>
+        <v>57.461114936844602</v>
       </c>
       <c r="N7">
-        <v>57.461114936844602</v>
+        <v>62.162595984131698</v>
       </c>
       <c r="O7">
-        <v>62.162595984131698</v>
+        <v>64.597061512726995</v>
       </c>
       <c r="P7">
-        <v>64.597061512726995</v>
+        <v>65.369907712281105</v>
       </c>
       <c r="Q7">
-        <v>65.369907712281105</v>
+        <v>67.070169351299995</v>
       </c>
       <c r="R7">
-        <v>67.070169351299995</v>
+        <v>67.392188601114199</v>
       </c>
       <c r="S7">
-        <v>67.392188601114199</v>
+        <v>66.458332776652995</v>
       </c>
       <c r="T7">
-        <v>66.458332776652995</v>
+        <v>66.806113566452396</v>
       </c>
       <c r="U7">
-        <v>66.806113566452396</v>
+        <v>67.823694395865203</v>
       </c>
       <c r="V7">
-        <v>67.823694395865203</v>
+        <v>69.414469489947393</v>
       </c>
       <c r="W7">
-        <v>69.414469489947393</v>
+        <v>71.816733093561297</v>
       </c>
       <c r="X7">
-        <v>71.816733093561297</v>
+        <v>74.276960162141705</v>
       </c>
       <c r="Y7">
-        <v>74.276960162141705</v>
+        <v>75.957900646171794</v>
       </c>
       <c r="Z7">
-        <v>75.957900646171794</v>
+        <v>77.696804595168203</v>
       </c>
       <c r="AA7">
-        <v>77.696804595168203</v>
+        <v>80.105508583778601</v>
       </c>
       <c r="AB7">
-        <v>80.105508583778601</v>
+        <v>81.483750972983103</v>
       </c>
       <c r="AC7">
-        <v>81.483750972983103</v>
+        <v>82.610818347333307</v>
       </c>
       <c r="AD7">
-        <v>82.610818347333307</v>
+        <v>84.265997291377701</v>
       </c>
       <c r="AE7">
-        <v>84.265997291377701</v>
+        <v>84.040583816508303</v>
       </c>
       <c r="AF7">
-        <v>84.040583816508303</v>
+        <v>84.054626858335794</v>
       </c>
       <c r="AG7">
-        <v>84.054626858335794</v>
+        <v>85.199134767275098</v>
       </c>
       <c r="AH7">
-        <v>85.199134767275098</v>
+        <v>86.048738797836904</v>
       </c>
       <c r="AI7">
-        <v>86.048738797836904</v>
+        <v>85.7117057939776</v>
       </c>
       <c r="AJ7">
-        <v>85.7117057939776</v>
+        <v>86.147040090629204</v>
       </c>
       <c r="AK7">
-        <v>86.147040090629204</v>
+        <v>87.579430357031399</v>
       </c>
       <c r="AL7">
-        <v>87.579430357031399</v>
+        <v>87.951736012462604</v>
       </c>
       <c r="AM7">
-        <v>87.951736012462604</v>
+        <v>88.798624842453705</v>
       </c>
       <c r="AN7">
-        <v>88.798624842453705</v>
+        <v>90.667729369300005</v>
       </c>
       <c r="AO7">
-        <v>90.667729369300005</v>
+        <v>96.676988610904004</v>
       </c>
       <c r="AP7">
-        <v>96.676988610904004</v>
+        <v>97.253879786213702</v>
       </c>
       <c r="AQ7">
-        <v>97.253879786213702</v>
+        <v>100</v>
       </c>
       <c r="AR7">
-        <v>100</v>
+        <v>105.24779339840499</v>
       </c>
       <c r="AS7">
-        <v>105.24779339840499</v>
+        <v>110.063514278795</v>
       </c>
       <c r="AT7">
-        <v>110.063514278795</v>
+        <v>112.659476898612</v>
       </c>
       <c r="AU7">
-        <v>112.659476898612</v>
+        <v>113.81440330709</v>
       </c>
       <c r="AV7">
-        <v>113.81440330709</v>
+        <v>113.219588558659</v>
       </c>
       <c r="AW7">
-        <v>113.219588558659</v>
+        <v>112.616956081526</v>
       </c>
       <c r="AX7">
-        <v>112.616956081526</v>
+        <v>113.265922901941</v>
       </c>
       <c r="AY7">
-        <v>113.265922901941</v>
+        <v>113.762730027133</v>
       </c>
       <c r="AZ7">
-        <v>113.762730027133</v>
-      </c>
-      <c r="BA7">
         <v>114.40578588194499</v>
       </c>
-      <c r="BB7" t="s">
+      <c r="BA7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1919,161 +1898,158 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
+      <c r="D8">
+        <v>4.2927666881304498</v>
       </c>
       <c r="E8">
-        <v>4.2927666881304498</v>
+        <v>3.2722782465528302</v>
       </c>
       <c r="F8">
-        <v>3.2722782465528302</v>
+        <v>6.1777600637704104</v>
       </c>
       <c r="G8">
-        <v>6.1777600637704104</v>
+        <v>11.0548048048048</v>
       </c>
       <c r="H8">
-        <v>11.0548048048048</v>
+        <v>9.14314686496534</v>
       </c>
       <c r="I8">
-        <v>9.14314686496534</v>
+        <v>5.7448126354908498</v>
       </c>
       <c r="J8">
-        <v>5.7448126354908498</v>
+        <v>6.5016839947283902</v>
       </c>
       <c r="K8">
-        <v>6.5016839947283902</v>
+        <v>7.6309638388560197</v>
       </c>
       <c r="L8">
-        <v>7.6309638388560197</v>
+        <v>11.2544711292795</v>
       </c>
       <c r="M8">
-        <v>11.2544711292795</v>
+        <v>13.549201974968399</v>
       </c>
       <c r="N8">
-        <v>13.549201974968399</v>
+        <v>10.3347153402771</v>
       </c>
       <c r="O8">
-        <v>10.3347153402771</v>
+        <v>6.1314270002749396</v>
       </c>
       <c r="P8">
-        <v>6.1314270002749396</v>
+        <v>3.2124352331606301</v>
       </c>
       <c r="Q8">
-        <v>3.2124352331606301</v>
+        <v>4.3005354752342697</v>
       </c>
       <c r="R8">
-        <v>4.3005354752342697</v>
+        <v>3.5456441520936899</v>
       </c>
       <c r="S8">
-        <v>3.5456441520936899</v>
+        <v>1.8980477223427501</v>
       </c>
       <c r="T8">
-        <v>1.8980477223427501</v>
+        <v>3.6645632175169101</v>
       </c>
       <c r="U8">
-        <v>3.6645632175169101</v>
+        <v>4.0777411074440799</v>
       </c>
       <c r="V8">
-        <v>4.0777411074440799</v>
+        <v>4.8270030300894904</v>
       </c>
       <c r="W8">
-        <v>4.8270030300894904</v>
+        <v>5.3979564399032203</v>
       </c>
       <c r="X8">
-        <v>5.3979564399032203</v>
+        <v>4.2349639645385304</v>
       </c>
       <c r="Y8">
-        <v>4.2349639645385304</v>
+        <v>3.0288196781496999</v>
       </c>
       <c r="Z8">
-        <v>3.0288196781496999</v>
+        <v>2.9516569663855399</v>
       </c>
       <c r="AA8">
-        <v>2.9516569663855399</v>
+        <v>2.6074415921546001</v>
       </c>
       <c r="AB8">
-        <v>2.6074415921546001</v>
+        <v>2.8054196885365501</v>
       </c>
       <c r="AC8">
-        <v>2.8054196885365501</v>
+        <v>2.9312041999343998</v>
       </c>
       <c r="AD8">
-        <v>2.9312041999343998</v>
+        <v>2.33768993730741</v>
       </c>
       <c r="AE8">
-        <v>2.33768993730741</v>
+        <v>1.5522790987436199</v>
       </c>
       <c r="AF8">
-        <v>1.5522790987436199</v>
+        <v>2.1880271969735801</v>
       </c>
       <c r="AG8">
-        <v>2.1880271969735801</v>
+        <v>3.3768572714993499</v>
       </c>
       <c r="AH8">
-        <v>3.3768572714993499</v>
+        <v>2.8261711188540199</v>
       </c>
       <c r="AI8">
-        <v>2.8261711188540199</v>
+        <v>1.5860316265060299</v>
       </c>
       <c r="AJ8">
-        <v>1.5860316265060299</v>
+        <v>2.2700949733611302</v>
       </c>
       <c r="AK8">
-        <v>2.2700949733611302</v>
+        <v>2.67723669309173</v>
       </c>
       <c r="AL8">
-        <v>2.67723669309173</v>
+        <v>3.3927468454954699</v>
       </c>
       <c r="AM8">
-        <v>3.3927468454954699</v>
+        <v>3.2259441007040701</v>
       </c>
       <c r="AN8">
-        <v>3.2259441007040701</v>
+        <v>2.8526724815013602</v>
       </c>
       <c r="AO8">
-        <v>2.8526724815013602</v>
+        <v>3.8391002966510102</v>
       </c>
       <c r="AP8">
-        <v>3.8391002966510102</v>
+        <v>-0.35554626629975</v>
       </c>
       <c r="AQ8">
-        <v>-0.35554626629975</v>
+        <v>1.64004344238989</v>
       </c>
       <c r="AR8">
-        <v>1.64004344238989</v>
+        <v>3.1568415686220601</v>
       </c>
       <c r="AS8">
-        <v>3.1568415686220601</v>
+        <v>2.0693372652605899</v>
       </c>
       <c r="AT8">
-        <v>2.0693372652605899</v>
+        <v>1.46483265562714</v>
       </c>
       <c r="AU8">
-        <v>1.46483265562714</v>
+        <v>1.62222297740821</v>
       </c>
       <c r="AV8">
-        <v>1.62222297740821</v>
+        <v>0.118627135552435</v>
       </c>
       <c r="AW8">
-        <v>0.118627135552435</v>
+        <v>1.26158320570537</v>
       </c>
       <c r="AX8">
-        <v>1.26158320570537</v>
+        <v>2.1301100036596301</v>
       </c>
       <c r="AY8">
-        <v>2.1301100036596301</v>
+        <v>2.4425832969281802</v>
       </c>
       <c r="AZ8">
-        <v>2.4425832969281802</v>
-      </c>
-      <c r="BA8">
         <v>1.81221007526015</v>
       </c>
-      <c r="BB8" t="s">
+      <c r="BA8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -2083,161 +2059,158 @@
       <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
+      <c r="D9">
+        <v>3.2933623777714303</v>
       </c>
       <c r="E9">
-        <v>3.2933623777714303</v>
+        <v>5.2588953577615456</v>
       </c>
       <c r="F9">
-        <v>5.2588953577615456</v>
+        <v>5.6457194703747291</v>
       </c>
       <c r="G9">
-        <v>5.6457194703747291</v>
+        <v>-0.54054652907490208</v>
       </c>
       <c r="H9">
-        <v>-0.54054652907490208</v>
+        <v>-0.2054640121342004</v>
       </c>
       <c r="I9">
-        <v>-0.2054640121342004</v>
+        <v>5.3881392265735144</v>
       </c>
       <c r="J9">
-        <v>5.3881392265735144</v>
+        <v>4.6241592068368931</v>
       </c>
       <c r="K9">
-        <v>4.6241592068368931</v>
+        <v>5.5353026932853311</v>
       </c>
       <c r="L9">
-        <v>5.5353026932853311</v>
+        <v>3.1661502709532101</v>
       </c>
       <c r="M9">
-        <v>3.1661502709532101</v>
+        <v>-0.256751930992138</v>
       </c>
       <c r="N9">
-        <v>-0.256751930992138</v>
+        <v>2.5377186978074633</v>
       </c>
       <c r="O9">
-        <v>2.5377186978074633</v>
+        <v>-1.8028744527117624</v>
       </c>
       <c r="P9">
-        <v>-1.8028744527117624</v>
+        <v>4.5839273156610147</v>
       </c>
       <c r="Q9">
-        <v>4.5839273156610147</v>
+        <v>7.2366199935738535</v>
       </c>
       <c r="R9">
-        <v>7.2366199935738535</v>
+        <v>4.1696559543024279</v>
       </c>
       <c r="S9">
-        <v>4.1696559543024279</v>
+        <v>3.462651712798916</v>
       </c>
       <c r="T9">
-        <v>3.462651712798916</v>
+        <v>3.4595725553488279</v>
       </c>
       <c r="U9">
-        <v>3.4595725553488279</v>
+        <v>4.1770463844437842</v>
       </c>
       <c r="V9">
-        <v>4.1770463844437842</v>
+        <v>3.6726563285104561</v>
       </c>
       <c r="W9">
-        <v>3.6726563285104561</v>
+        <v>1.8859603230941815</v>
       </c>
       <c r="X9">
-        <v>1.8859603230941815</v>
+        <v>-0.10825910527866256</v>
       </c>
       <c r="Y9">
-        <v>-0.10825910527866256</v>
+        <v>3.5224424938664356</v>
       </c>
       <c r="Z9">
-        <v>3.5224424938664356</v>
+        <v>2.7528443268801226</v>
       </c>
       <c r="AA9">
-        <v>2.7528443268801226</v>
+        <v>4.0288390635428044</v>
       </c>
       <c r="AB9">
-        <v>4.0288390635428044</v>
+        <v>2.6842871324197688</v>
       </c>
       <c r="AC9">
-        <v>2.6842871324197688</v>
+        <v>3.7725013192651886</v>
       </c>
       <c r="AD9">
-        <v>3.7725013192651886</v>
+        <v>4.4472163427340803</v>
       </c>
       <c r="AE9">
-        <v>4.4472163427340803</v>
+        <v>4.4814075545120744</v>
       </c>
       <c r="AF9">
-        <v>4.4814075545120744</v>
+        <v>4.7532359887971722</v>
       </c>
       <c r="AG9">
-        <v>4.7532359887971722</v>
+        <v>4.1274840135585293</v>
       </c>
       <c r="AH9">
-        <v>4.1274840135585293</v>
+        <v>0.9983407946564995</v>
       </c>
       <c r="AI9">
-        <v>0.9983407946564995</v>
+        <v>1.7416952497298013</v>
       </c>
       <c r="AJ9">
-        <v>1.7416952497298013</v>
+        <v>2.8612107674102418</v>
       </c>
       <c r="AK9">
-        <v>2.8612107674102418</v>
+        <v>3.7988911266239285</v>
       </c>
       <c r="AL9">
-        <v>3.7988911266239285</v>
+        <v>3.5132137966530195</v>
       </c>
       <c r="AM9">
-        <v>3.5132137966530195</v>
+        <v>2.8549722917001503</v>
       </c>
       <c r="AN9">
-        <v>2.8549722917001503</v>
+        <v>1.8761714584669278</v>
       </c>
       <c r="AO9">
-        <v>1.8761714584669278</v>
+        <v>-0.136579805460741</v>
       </c>
       <c r="AP9">
-        <v>-0.136579805460741</v>
+        <v>-2.5367570658566478</v>
       </c>
       <c r="AQ9">
-        <v>-2.5367570658566478</v>
+        <v>2.5637665587658063</v>
       </c>
       <c r="AR9">
-        <v>2.5637665587658063</v>
+        <v>1.5508355056815617</v>
       </c>
       <c r="AS9">
-        <v>1.5508355056815617</v>
+        <v>2.2495458523699341</v>
       </c>
       <c r="AT9">
-        <v>2.2495458523699341</v>
+        <v>1.8420810710110089</v>
       </c>
       <c r="AU9">
-        <v>1.8420810710110089</v>
+        <v>2.4519730353603393</v>
       </c>
       <c r="AV9">
-        <v>2.4519730353603393</v>
+        <v>2.8809104660521854</v>
       </c>
       <c r="AW9">
-        <v>2.8809104660521854</v>
+        <v>1.5672151699786383</v>
       </c>
       <c r="AX9">
-        <v>1.5672151699786383</v>
+        <v>2.2170103303188426</v>
       </c>
       <c r="AY9">
-        <v>2.2170103303188426</v>
+        <v>2.9273227282108536</v>
       </c>
       <c r="AZ9">
-        <v>2.9273227282108536</v>
-      </c>
-      <c r="BA9">
         <v>2.3335774919428758</v>
       </c>
-      <c r="BB9" t="s">
+      <c r="BA9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -2245,124 +2218,124 @@
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>11</v>
+        <v>121</v>
+      </c>
+      <c r="D10">
+        <v>5.7233333333333301</v>
       </c>
       <c r="E10">
-        <v>5.7233333333333301</v>
+        <v>5.2483333333333304</v>
       </c>
       <c r="F10">
-        <v>5.2483333333333304</v>
+        <v>8.0216666666666701</v>
       </c>
       <c r="G10">
-        <v>8.0216666666666701</v>
+        <v>10.7983333333333</v>
       </c>
       <c r="H10">
-        <v>10.7983333333333</v>
+        <v>7.8624999999999998</v>
       </c>
       <c r="I10">
-        <v>7.8624999999999998</v>
+        <v>6.84</v>
       </c>
       <c r="J10">
-        <v>6.84</v>
+        <v>6.8241666666666703</v>
       </c>
       <c r="K10">
-        <v>6.8241666666666703</v>
+        <v>9.0566666666666702</v>
       </c>
       <c r="L10">
-        <v>9.0566666666666702</v>
+        <v>12.6658333333333</v>
       </c>
       <c r="M10">
-        <v>12.6658333333333</v>
+        <v>15.265833333333299</v>
       </c>
       <c r="N10">
-        <v>15.265833333333299</v>
+        <v>18.87</v>
       </c>
       <c r="O10">
-        <v>18.87</v>
+        <v>14.8608333333333</v>
       </c>
       <c r="P10">
-        <v>14.8608333333333</v>
+        <v>10.794166666666699</v>
       </c>
       <c r="Q10">
-        <v>10.794166666666699</v>
+        <v>12.0425</v>
       </c>
       <c r="R10">
-        <v>12.0425</v>
+        <v>9.93333333333333</v>
       </c>
       <c r="S10">
-        <v>9.93333333333333</v>
+        <v>8.3324999999999996</v>
       </c>
       <c r="T10">
-        <v>8.3324999999999996</v>
+        <v>8.2033333333333296</v>
       </c>
       <c r="U10">
-        <v>8.2033333333333296</v>
+        <v>9.3149999999999995</v>
       </c>
       <c r="V10">
-        <v>9.3149999999999995</v>
+        <v>10.873333333333299</v>
       </c>
       <c r="W10">
-        <v>10.873333333333299</v>
+        <v>10.009166666666699</v>
       </c>
       <c r="X10">
-        <v>10.009166666666699</v>
+        <v>8.4633333333333294</v>
       </c>
       <c r="Y10">
-        <v>8.4633333333333294</v>
+        <v>6.2516666666666696</v>
       </c>
       <c r="Z10">
-        <v>6.2516666666666696</v>
+        <v>6</v>
       </c>
       <c r="AA10">
-        <v>6</v>
+        <v>7.1383333333333301</v>
       </c>
       <c r="AB10">
-        <v>7.1383333333333301</v>
+        <v>8.8291666666666693</v>
       </c>
       <c r="AC10">
-        <v>8.8291666666666693</v>
+        <v>8.2708333333333304</v>
       </c>
       <c r="AD10">
-        <v>8.2708333333333304</v>
+        <v>8.44166666666667</v>
       </c>
       <c r="AE10">
-        <v>8.44166666666667</v>
+        <v>8.3541666666666696</v>
       </c>
       <c r="AF10">
-        <v>8.3541666666666696</v>
+        <v>7.9941666666666702</v>
       </c>
       <c r="AG10">
-        <v>7.9941666666666702</v>
+        <v>9.2333333333333307</v>
       </c>
       <c r="AH10">
-        <v>9.2333333333333307</v>
+        <v>6.9216666666666704</v>
       </c>
       <c r="AI10">
-        <v>6.9216666666666704</v>
+        <v>4.6749999999999998</v>
       </c>
       <c r="AJ10">
-        <v>4.6749999999999998</v>
+        <v>4.1224999999999996</v>
       </c>
       <c r="AK10">
-        <v>4.1224999999999996</v>
+        <v>4.34</v>
       </c>
       <c r="AL10">
-        <v>4.34</v>
+        <v>6.1891666666666696</v>
       </c>
       <c r="AM10">
-        <v>6.1891666666666696</v>
+        <v>7.9574999999999996</v>
       </c>
       <c r="AN10">
-        <v>7.9574999999999996</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="AO10">
-        <v>8.0500000000000007</v>
+        <v>5.0875000000000004</v>
       </c>
       <c r="AP10">
-        <v>5.0875000000000004</v>
+        <v>3.25</v>
       </c>
       <c r="AQ10">
         <v>3.25</v>
@@ -2380,28 +2353,25 @@
         <v>3.25</v>
       </c>
       <c r="AV10">
-        <v>3.25</v>
+        <v>3.26</v>
       </c>
       <c r="AW10">
-        <v>3.26</v>
+        <v>3.5116666666666698</v>
       </c>
       <c r="AX10">
-        <v>3.5116666666666698</v>
+        <v>4.0966666666666702</v>
       </c>
       <c r="AY10">
-        <v>4.0966666666666702</v>
+        <v>4.9041666666666703</v>
       </c>
       <c r="AZ10">
-        <v>4.9041666666666703</v>
-      </c>
-      <c r="BA10">
         <v>5.2824999999999998</v>
       </c>
-      <c r="BB10" t="s">
+      <c r="BA10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -2411,161 +2381,158 @@
       <c r="C11" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>90</v>
+      <c r="D11">
+        <v>0.62261540444325281</v>
       </c>
       <c r="E11">
-        <v>0.62261540444325281</v>
+        <v>0.88721768829034209</v>
       </c>
       <c r="F11">
-        <v>0.88721768829034209</v>
+        <v>2.4097323357542084</v>
       </c>
       <c r="G11">
-        <v>2.4097323357542084</v>
+        <v>1.6510697048529048</v>
       </c>
       <c r="H11">
-        <v>1.6510697048529048</v>
+        <v>-1.2814270331490738</v>
       </c>
       <c r="I11">
-        <v>-1.2814270331490738</v>
+        <v>1.2668915930679947</v>
       </c>
       <c r="J11">
-        <v>1.2668915930679947</v>
+        <v>0.5750747577071269</v>
       </c>
       <c r="K11">
-        <v>0.5750747577071269</v>
+        <v>1.8899011034261353</v>
       </c>
       <c r="L11">
-        <v>1.8899011034261353</v>
+        <v>4.0345130977971531</v>
       </c>
       <c r="M11">
-        <v>4.0345130977971531</v>
+        <v>5.7164283275688605</v>
       </c>
       <c r="N11">
-        <v>5.7164283275688605</v>
+        <v>8.5945852911559957</v>
       </c>
       <c r="O11">
-        <v>8.5945852911559957</v>
+        <v>8.1773954397589748</v>
       </c>
       <c r="P11">
-        <v>8.1773954397589748</v>
+        <v>6.6181744504164133</v>
       </c>
       <c r="Q11">
-        <v>6.6181744504164133</v>
+        <v>8.1410748438774352</v>
       </c>
       <c r="R11">
-        <v>8.1410748438774352</v>
+        <v>6.563326293402886</v>
       </c>
       <c r="S11">
-        <v>6.563326293402886</v>
+        <v>6.1938661585148367</v>
       </c>
       <c r="T11">
-        <v>6.1938661585148367</v>
+        <v>5.5925650802053397</v>
       </c>
       <c r="U11">
-        <v>5.5925650802053397</v>
+        <v>5.5903670918095481</v>
       </c>
       <c r="V11">
-        <v>5.5903670918095481</v>
+        <v>6.6906953418547985</v>
       </c>
       <c r="W11">
-        <v>6.6906953418547985</v>
+        <v>6.0397443767060164</v>
       </c>
       <c r="X11">
-        <v>6.0397443767060164</v>
+        <v>4.9153524496992178</v>
       </c>
       <c r="Y11">
-        <v>4.9153524496992178</v>
+        <v>3.8842400162985626</v>
       </c>
       <c r="Z11">
-        <v>3.8842400162985626</v>
+        <v>3.5466887290514442</v>
       </c>
       <c r="AA11">
-        <v>3.5466887290514442</v>
+        <v>4.8983561373900093</v>
       </c>
       <c r="AB11">
-        <v>4.8983561373900093</v>
+        <v>6.5940689003308792</v>
       </c>
       <c r="AC11">
-        <v>6.5940689003308792</v>
+        <v>6.3240079486778695</v>
       </c>
       <c r="AD11">
-        <v>6.3240079486778695</v>
+        <v>6.6034070387998369</v>
       </c>
       <c r="AE11">
-        <v>6.6034070387998369</v>
+        <v>7.1481918741720474</v>
       </c>
       <c r="AF11">
-        <v>7.1481918741720474</v>
+        <v>6.4571349132677751</v>
       </c>
       <c r="AG11">
-        <v>6.4571349132677751</v>
+        <v>6.8448441841136436</v>
       </c>
       <c r="AH11">
-        <v>6.8448441841136436</v>
+        <v>4.6267568669171757</v>
       </c>
       <c r="AI11">
-        <v>4.6267568669171757</v>
+        <v>3.0450711829911081</v>
       </c>
       <c r="AJ11">
-        <v>3.0450711829911081</v>
+        <v>2.2241011221949027</v>
       </c>
       <c r="AK11">
-        <v>2.2241011221949027</v>
+        <v>1.6045889376330591</v>
       </c>
       <c r="AL11">
-        <v>1.6045889376330591</v>
+        <v>2.9813567792705378</v>
       </c>
       <c r="AM11">
-        <v>2.9813567792705378</v>
+        <v>4.7864476474923201</v>
       </c>
       <c r="AN11">
-        <v>4.7864476474923201</v>
+        <v>5.2234058896542965</v>
       </c>
       <c r="AO11">
-        <v>5.2234058896542965</v>
+        <v>3.0824112914405557</v>
       </c>
       <c r="AP11">
-        <v>3.0824112914405557</v>
+        <v>2.4688288961340259</v>
       </c>
       <c r="AQ11">
-        <v>2.4688288961340259</v>
+        <v>2.06073670900187</v>
       </c>
       <c r="AR11">
-        <v>2.06073670900187</v>
+        <v>1.1373383201857636</v>
       </c>
       <c r="AS11">
-        <v>1.1373383201857636</v>
+        <v>1.3070831127829725</v>
       </c>
       <c r="AT11">
-        <v>1.3070831127829725</v>
+        <v>1.4692992871518793</v>
       </c>
       <c r="AU11">
-        <v>1.4692992871518793</v>
+        <v>1.3328918416429982</v>
       </c>
       <c r="AV11">
-        <v>1.3328918416429982</v>
+        <v>2.1674805681731675</v>
       </c>
       <c r="AW11">
-        <v>2.1674805681731675</v>
+        <v>2.3919842868373693</v>
       </c>
       <c r="AX11">
-        <v>2.3919842868373693</v>
+        <v>2.154928727590343</v>
       </c>
       <c r="AY11">
-        <v>2.154928727590343</v>
+        <v>2.4858171056628122</v>
       </c>
       <c r="AZ11">
-        <v>2.4858171056628122</v>
-      </c>
-      <c r="BA11">
         <v>3.4781998344735476</v>
       </c>
-      <c r="BB11" t="s">
+      <c r="BA11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -2575,8 +2542,8 @@
       <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>109</v>
+      <c r="D12" t="s">
+        <v>31</v>
       </c>
       <c r="E12" t="s">
         <v>31</v>
@@ -2602,134 +2569,131 @@
       <c r="L12" t="s">
         <v>31</v>
       </c>
-      <c r="M12" t="s">
-        <v>31</v>
+      <c r="M12">
+        <v>105.708339604728</v>
       </c>
       <c r="N12">
-        <v>105.708339604728</v>
+        <v>116.54431283855899</v>
       </c>
       <c r="O12">
-        <v>116.54431283855899</v>
+        <v>130.362852944102</v>
       </c>
       <c r="P12">
-        <v>130.362852944102</v>
+        <v>136.471991403121</v>
       </c>
       <c r="Q12">
-        <v>136.471991403121</v>
+        <v>144.880762044709</v>
       </c>
       <c r="R12">
-        <v>144.880762044709</v>
+        <v>150.00403879303499</v>
       </c>
       <c r="S12">
-        <v>150.00403879303499</v>
+        <v>125.962520194588</v>
       </c>
       <c r="T12">
-        <v>125.962520194588</v>
+        <v>113.400265890299</v>
       </c>
       <c r="U12">
-        <v>113.400265890299</v>
+        <v>107.227893989462</v>
       </c>
       <c r="V12">
-        <v>107.227893989462</v>
+        <v>110.883158025152</v>
       </c>
       <c r="W12">
-        <v>110.883158025152</v>
+        <v>105.84133590606</v>
       </c>
       <c r="X12">
-        <v>105.84133590606</v>
+        <v>104.37621551829</v>
       </c>
       <c r="Y12">
-        <v>104.37621551829</v>
+        <v>101.786128655822</v>
       </c>
       <c r="Z12">
-        <v>101.786128655822</v>
+        <v>104.753376315125</v>
       </c>
       <c r="AA12">
-        <v>104.753376315125</v>
+        <v>104.1940532717</v>
       </c>
       <c r="AB12">
-        <v>104.1940532717</v>
+        <v>100.74755539504601</v>
       </c>
       <c r="AC12">
-        <v>100.74755539504601</v>
+        <v>103.743034826795</v>
       </c>
       <c r="AD12">
-        <v>103.743034826795</v>
+        <v>108.872395516222</v>
       </c>
       <c r="AE12">
-        <v>108.872395516222</v>
+        <v>116.71018086725</v>
       </c>
       <c r="AF12">
-        <v>116.71018086725</v>
+        <v>115.561499235711</v>
       </c>
       <c r="AG12">
-        <v>115.561499235711</v>
+        <v>119.465783140266</v>
       </c>
       <c r="AH12">
-        <v>119.465783140266</v>
+        <v>126.22677850337701</v>
       </c>
       <c r="AI12">
-        <v>126.22677850337701</v>
+        <v>125.916647298371</v>
       </c>
       <c r="AJ12">
-        <v>125.916647298371</v>
+        <v>117.99469441646499</v>
       </c>
       <c r="AK12">
-        <v>117.99469441646499</v>
+        <v>112.398884645763</v>
       </c>
       <c r="AL12">
-        <v>112.398884645763</v>
+        <v>110.840929967704</v>
       </c>
       <c r="AM12">
-        <v>110.840929967704</v>
+        <v>109.924177794513</v>
       </c>
       <c r="AN12">
-        <v>109.924177794513</v>
+        <v>104.893470558422</v>
       </c>
       <c r="AO12">
-        <v>104.893470558422</v>
+        <v>100.450148993236</v>
       </c>
       <c r="AP12">
-        <v>100.450148993236</v>
+        <v>104.699158946605</v>
       </c>
       <c r="AQ12">
-        <v>104.699158946605</v>
+        <v>100</v>
       </c>
       <c r="AR12">
-        <v>100</v>
+        <v>95.011482054544004</v>
       </c>
       <c r="AS12">
-        <v>95.011482054544004</v>
+        <v>97.375250080383694</v>
       </c>
       <c r="AT12">
-        <v>97.375250080383694</v>
+        <v>97.537237973556103</v>
       </c>
       <c r="AU12">
-        <v>97.537237973556103</v>
+        <v>99.177517397522706</v>
       </c>
       <c r="AV12">
-        <v>99.177517397522706</v>
+        <v>109.87693689369399</v>
       </c>
       <c r="AW12">
-        <v>109.87693689369399</v>
+        <v>114.34925019165399</v>
       </c>
       <c r="AX12">
-        <v>114.34925019165399</v>
+        <v>114.07471654296199</v>
       </c>
       <c r="AY12">
-        <v>114.07471654296199</v>
+        <v>112.987226305809</v>
       </c>
       <c r="AZ12">
-        <v>112.987226305809</v>
-      </c>
-      <c r="BA12">
         <v>116.12130129389401</v>
       </c>
-      <c r="BB12" t="s">
+      <c r="BA12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -2737,182 +2701,178 @@
         <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="D13">
+        <v>18.569431482657698</v>
       </c>
       <c r="E13">
-        <v>18.569431482657698</v>
+        <v>19.1770749495732</v>
       </c>
       <c r="F13">
-        <v>19.1770749495732</v>
+        <v>20.3617886272073</v>
       </c>
       <c r="G13">
-        <v>20.3617886272073</v>
+        <v>22.612744614712</v>
       </c>
       <c r="H13">
-        <v>22.612744614712</v>
+        <v>24.680261065034699</v>
       </c>
       <c r="I13">
-        <v>24.680261065034699</v>
+        <v>26.098095821170901</v>
       </c>
       <c r="J13">
-        <v>26.098095821170901</v>
+        <v>27.794911540104899</v>
       </c>
       <c r="K13">
-        <v>27.794911540104899</v>
+        <v>29.915931188772301</v>
       </c>
       <c r="L13">
-        <v>29.915931188772301</v>
+        <v>33.282811027467801</v>
       </c>
       <c r="M13">
-        <v>33.282811027467801</v>
+        <v>37.792366316526497</v>
       </c>
       <c r="N13">
-        <v>37.792366316526497</v>
+        <v>41.698099795694198</v>
       </c>
       <c r="O13">
-        <v>41.698099795694198</v>
+        <v>44.254788345168997</v>
       </c>
       <c r="P13">
-        <v>44.254788345168997</v>
+        <v>45.6764447583299</v>
       </c>
       <c r="Q13">
-        <v>45.6764447583299</v>
+        <v>47.640776468987603</v>
       </c>
       <c r="R13">
-        <v>47.640776468987603</v>
+        <v>49.329948873872297</v>
       </c>
       <c r="S13">
-        <v>49.329948873872297</v>
+        <v>50.266254844905703</v>
       </c>
       <c r="T13">
-        <v>50.266254844905703</v>
+        <v>52.108293530775398</v>
       </c>
       <c r="U13">
-        <v>52.108293530775398</v>
+        <v>54.233134836467499</v>
       </c>
       <c r="V13">
-        <v>54.233134836467499</v>
+        <v>56.850969898336302</v>
       </c>
       <c r="W13">
-        <v>56.850969898336302</v>
+        <v>59.919760489110999</v>
       </c>
       <c r="X13">
-        <v>59.919760489110999</v>
+        <v>62.457340753462603</v>
       </c>
       <c r="Y13">
-        <v>62.457340753462603</v>
+        <v>64.349060980652496</v>
       </c>
       <c r="Z13">
-        <v>64.349060980652496</v>
+        <v>66.248424521891593</v>
       </c>
       <c r="AA13">
-        <v>66.248424521891593</v>
+        <v>67.9758134970226</v>
       </c>
       <c r="AB13">
-        <v>67.9758134970226</v>
+        <v>69.882820352310901</v>
       </c>
       <c r="AC13">
-        <v>69.882820352310901</v>
+        <v>71.931228517510505</v>
       </c>
       <c r="AD13">
-        <v>71.931228517510505</v>
+        <v>73.612757608345902</v>
       </c>
       <c r="AE13">
-        <v>73.612757608345902</v>
+        <v>74.755433058709102</v>
       </c>
       <c r="AF13">
-        <v>74.755433058709102</v>
+        <v>76.391102265249003</v>
       </c>
       <c r="AG13">
-        <v>76.391102265249003</v>
+        <v>78.9707207568716</v>
       </c>
       <c r="AH13">
-        <v>78.9707207568716</v>
+        <v>81.202568459253101</v>
       </c>
       <c r="AI13">
-        <v>81.202568459253101</v>
+        <v>82.490466876552105</v>
       </c>
       <c r="AJ13">
-        <v>82.490466876552105</v>
+        <v>84.363078818618803</v>
       </c>
       <c r="AK13">
-        <v>84.363078818618803</v>
+        <v>86.621678120172803</v>
       </c>
       <c r="AL13">
-        <v>86.621678120172803</v>
+        <v>89.560532372110202</v>
       </c>
       <c r="AM13">
-        <v>89.560532372110202</v>
+        <v>92.449705082727405</v>
       </c>
       <c r="AN13">
-        <v>92.449705082727405</v>
+        <v>95.086992378851505</v>
       </c>
       <c r="AO13">
-        <v>95.086992378851505</v>
+        <v>98.737477385344604</v>
       </c>
       <c r="AP13">
-        <v>98.737477385344604</v>
+        <v>98.386419971062395</v>
       </c>
       <c r="AQ13">
-        <v>98.386419971062395</v>
+        <v>100</v>
       </c>
       <c r="AR13">
-        <v>100</v>
+        <v>103.156841568622</v>
       </c>
       <c r="AS13">
-        <v>103.156841568622</v>
+        <v>105.29150453286699</v>
       </c>
       <c r="AT13">
-        <v>105.29150453286699</v>
+        <v>106.83384887486601</v>
       </c>
       <c r="AU13">
-        <v>106.83384887486601</v>
+        <v>108.566932118964</v>
       </c>
       <c r="AV13">
-        <v>108.566932118964</v>
+        <v>108.69572196069301</v>
       </c>
       <c r="AW13">
-        <v>108.69572196069301</v>
+        <v>110.06700893427001</v>
       </c>
       <c r="AX13">
-        <v>110.06700893427001</v>
+        <v>112.411557302308</v>
       </c>
       <c r="AY13">
-        <v>112.411557302308</v>
+        <v>115.15730322479099</v>
       </c>
       <c r="AZ13">
-        <v>115.15730322479099</v>
-      </c>
-      <c r="BA13">
         <v>117.244195476228</v>
       </c>
-      <c r="BB13" t="s">
+      <c r="BA13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="C14" t="s">
+        <v>124</v>
+      </c>
     </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
-      <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
-      <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>73</v>
       </c>
@@ -2942,13 +2902,13 @@
         <v>53</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>61</v>
@@ -2957,13 +2917,13 @@
         <v>74</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>0</v>
@@ -2972,7 +2932,7 @@
         <v>50</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -3019,7 +2979,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
@@ -3049,7 +3009,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>60</v>
@@ -3064,7 +3024,7 @@
         <v>83</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>32</v>
@@ -3078,7 +3038,7 @@
         <v>52</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>8</v>
@@ -3092,7 +3052,7 @@
         <v>60</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>2</v>
@@ -3101,7 +3061,7 @@
         <v>83</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>32</v>
@@ -3115,7 +3075,7 @@
         <v>52</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>8</v>
@@ -3135,10 +3095,10 @@
         <v>88</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>32</v>
@@ -3149,7 +3109,7 @@
         <v>66</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2" t="s">
@@ -3173,7 +3133,7 @@
         <v>83</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>32</v>
@@ -3189,7 +3149,7 @@
         <v>52</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>8</v>
@@ -3197,7 +3157,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>60</v>
@@ -3236,16 +3196,16 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>83</v>
@@ -3261,7 +3221,7 @@
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>75</v>

</xml_diff>